<commit_message>
updated run_configs and data - incorporates changes to CryoGrid_pytools - moved stratigraphy to data/stratigraphy.py - run_config...py now has multiple run configs
</commit_message>
<xml_diff>
--- a/templates/run_config.xlsx
+++ b/templates/run_config.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Git/CryoGrid-run-manager/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luke/Work/PAMIR/CryoGrid-run-manager/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8788684E-AF1E-ED46-96CA-15DDD8EBEFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC3731A-D800-3E4D-BCB5-730DC2A0856A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="880" windowWidth="22360" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="560" windowWidth="22360" windowHeight="28180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simplest" sheetId="6" r:id="rId1"/>
-    <sheet name="notes" sheetId="3" r:id="rId2"/>
-    <sheet name="original" sheetId="2" r:id="rId3"/>
+    <sheet name="stratigraphies" sheetId="7" r:id="rId2"/>
+    <sheet name="notes" sheetId="3" r:id="rId3"/>
+    <sheet name="original" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2948" uniqueCount="506">
   <si>
     <t>-------------------</t>
   </si>
@@ -1426,13 +1427,145 @@
   </si>
   <si>
     <t>surface_classes.tif</t>
+  </si>
+  <si>
+    <t>### vegetated sediments</t>
+  </si>
+  <si>
+    <t>permeability</t>
+  </si>
+  <si>
+    <t>litter layer, very high water/ice at surface, high porosity</t>
+  </si>
+  <si>
+    <t>sediment layer</t>
+  </si>
+  <si>
+    <t>"bedock" layer</t>
+  </si>
+  <si>
+    <t>Litter layer, low water ice contents</t>
+  </si>
+  <si>
+    <t>second thin layer, high porosity</t>
+  </si>
+  <si>
+    <t>water/ice + sediment layer</t>
+  </si>
+  <si>
+    <t>dryer below</t>
+  </si>
+  <si>
+    <t>Bedrock</t>
+  </si>
+  <si>
+    <t>litter layer, low water/ice content, high organic content</t>
+  </si>
+  <si>
+    <t>high-er water/ice content</t>
+  </si>
+  <si>
+    <t>dryer sediment below</t>
+  </si>
+  <si>
+    <t>bedrock layer</t>
+  </si>
+  <si>
+    <t>same as before but dryer</t>
+  </si>
+  <si>
+    <t>### DEBRIS (coarse-blocky stratigraphies, based on talus slope and moraine geophysical profiles)</t>
+  </si>
+  <si>
+    <t>thin layer, very high porosity</t>
+  </si>
+  <si>
+    <t>moderate ice content</t>
+  </si>
+  <si>
+    <t>a little less water/ice</t>
+  </si>
+  <si>
+    <t>bedrock</t>
+  </si>
+  <si>
+    <t>slightly humid debris</t>
+  </si>
+  <si>
+    <t>ice-filled core (ice-rich moraine for example)</t>
+  </si>
+  <si>
+    <t>Ice-rock mix</t>
+  </si>
+  <si>
+    <t>porous and dry</t>
+  </si>
+  <si>
+    <t>low ice /dry</t>
+  </si>
+  <si>
+    <t>sediment/blocky</t>
+  </si>
+  <si>
+    <t>### BEDROCK (not geophysical data, just basic bedrock after Sebastians stratigraphies --&gt; maybe different bedrock based on geological map --&gt; different thermal conductivity..)</t>
+  </si>
+  <si>
+    <t>pure bedrock</t>
+  </si>
+  <si>
+    <t>dry sediment layer above bedrock</t>
+  </si>
+  <si>
+    <t>Bedrock, small sediment layer above</t>
+  </si>
+  <si>
+    <t>### FINE-GRAINED SEDIMENTS (no vegetation, otherwise similar to vegetated sediments)</t>
+  </si>
+  <si>
+    <t>water filled at surface</t>
+  </si>
+  <si>
+    <t>less waterice</t>
+  </si>
+  <si>
+    <t>lower field capacity</t>
+  </si>
+  <si>
+    <t>shallower water/ce rich layer</t>
+  </si>
+  <si>
+    <t>water/ice a bit lower</t>
+  </si>
+  <si>
+    <t>in general dryer conditions</t>
+  </si>
+  <si>
+    <t>### ROCK GLACIERS</t>
+  </si>
+  <si>
+    <t>blocks, air-filled, no water/ice, high porosity, high drainage</t>
+  </si>
+  <si>
+    <t>blocks, air-filled, little water/ice ,high porosity, high drainage</t>
+  </si>
+  <si>
+    <t>ice core, no  air, very low drainage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bedrock </t>
+  </si>
+  <si>
+    <t>ice core, no  air, very low drainage, more ice than in 11</t>
+  </si>
+  <si>
+    <t>ice core, less ice, more mineral content, a bit of water retention possible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1647,8 +1780,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1669,6 +1828,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1758,7 +1947,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1843,6 +2032,30 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="30" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="30" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="30" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="30" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2127,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC02FF78-754A-6749-899C-79A6381DAB46}">
   <dimension ref="A1:T535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A257" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C346" sqref="C346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5557,7 +5770,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="348" spans="1:8" ht="19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A348" s="19" t="s">
         <v>54</v>
       </c>
@@ -5568,7 +5781,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" s="4" t="s">
         <v>232</v>
       </c>
@@ -5576,7 +5789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>206</v>
       </c>
@@ -5584,7 +5797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>55</v>
       </c>
@@ -5604,7 +5817,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B352">
         <v>0</v>
       </c>
@@ -5619,7 +5832,7 @@
         <v>&gt; GROUND_freeW_bucketW_seb_snow</v>
       </c>
     </row>
-    <row r="353" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B353">
         <v>1</v>
       </c>
@@ -5634,7 +5847,7 @@
         <v>&gt; GROUND_freezeC_bucketW_seb_snow</v>
       </c>
     </row>
-    <row r="354" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B354">
         <v>2.5</v>
       </c>
@@ -5649,12 +5862,12 @@
         <v>&gt; GROUND_freeW_seb</v>
       </c>
     </row>
-    <row r="355" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B355" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="356" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>60</v>
       </c>
@@ -5666,7 +5879,7 @@
         <v>&gt; SNOW_crocus_bucketW_seb</v>
       </c>
     </row>
-    <row r="357" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>61</v>
       </c>
@@ -5674,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>62</v>
       </c>
@@ -5685,7 +5898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="359" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>63</v>
       </c>
@@ -5696,14 +5909,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="360" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="361" spans="1:20" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="362" spans="1:20" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="363" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A363" s="19" t="s">
         <v>64</v>
       </c>
@@ -5711,7 +5922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="364" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A364" s="4" t="s">
         <v>205</v>
       </c>
@@ -5722,7 +5933,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="365" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>206</v>
       </c>
@@ -5735,7 +5946,7 @@
       <c r="S365" s="2"/>
       <c r="T365" s="2"/>
     </row>
-    <row r="366" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>65</v>
       </c>
@@ -5769,7 +5980,7 @@
       <c r="S366" s="2"/>
       <c r="T366" s="2"/>
     </row>
-    <row r="367" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B367" s="2">
         <v>0</v>
       </c>
@@ -5797,7 +6008,7 @@
       <c r="S367" s="2"/>
       <c r="T367" s="2"/>
     </row>
-    <row r="368" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B368" s="2">
         <v>1</v>
       </c>
@@ -5825,7 +6036,7 @@
       <c r="S368" s="2"/>
       <c r="T368" s="2"/>
     </row>
-    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B369" s="2">
         <v>2.5</v>
       </c>
@@ -5848,7 +6059,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B370" s="2" t="s">
         <v>26</v>
       </c>
@@ -5858,7 +6069,7 @@
       <c r="F370" s="2"/>
       <c r="G370" s="2"/>
     </row>
-    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>7</v>
       </c>
@@ -7898,6 +8109,3670 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267834D4-E050-2145-8D10-AF4F7582CBDF}">
+  <dimension ref="A1:K176"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E157" sqref="E157"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="10" width="8.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="67" t="s">
+        <v>488</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+    </row>
+    <row r="2" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="61">
+        <v>1</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>489</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H5" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J5" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="61"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="69"/>
+      <c r="B6" s="69">
+        <v>0</v>
+      </c>
+      <c r="C6" s="69">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="69">
+        <v>0.97</v>
+      </c>
+      <c r="E6" s="69">
+        <v>0</v>
+      </c>
+      <c r="F6" s="69">
+        <v>0.03</v>
+      </c>
+      <c r="G6" s="69">
+        <v>1</v>
+      </c>
+      <c r="H6" s="70">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I6" s="69">
+        <v>0</v>
+      </c>
+      <c r="J6" s="69"/>
+      <c r="K6" s="71" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="61"/>
+      <c r="B7" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" s="61">
+        <v>2</v>
+      </c>
+      <c r="C11" s="61" t="s">
+        <v>490</v>
+      </c>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I12" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J12" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="69"/>
+      <c r="B13" s="69">
+        <v>0</v>
+      </c>
+      <c r="C13" s="69">
+        <v>0.05</v>
+      </c>
+      <c r="D13" s="69">
+        <v>0.85</v>
+      </c>
+      <c r="E13" s="69">
+        <v>0</v>
+      </c>
+      <c r="F13" s="69">
+        <v>0.05</v>
+      </c>
+      <c r="G13" s="69">
+        <v>1</v>
+      </c>
+      <c r="H13" s="70">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I13" s="69">
+        <v>0</v>
+      </c>
+      <c r="J13" s="71"/>
+      <c r="K13" s="69"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="69"/>
+      <c r="B14" s="69">
+        <v>0.3</v>
+      </c>
+      <c r="C14" s="69">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="69">
+        <v>0.97</v>
+      </c>
+      <c r="E14" s="69">
+        <v>0</v>
+      </c>
+      <c r="F14" s="69">
+        <v>0.03</v>
+      </c>
+      <c r="G14" s="69">
+        <v>1</v>
+      </c>
+      <c r="H14" s="70">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I14" s="69">
+        <v>0</v>
+      </c>
+      <c r="J14" s="69"/>
+      <c r="K14" s="71" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="61"/>
+      <c r="B15" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+    </row>
+    <row r="20" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="73" t="s">
+        <v>499</v>
+      </c>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B23" s="61">
+        <v>11</v>
+      </c>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H24" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I24" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J24" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="61"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="75"/>
+      <c r="B25" s="75">
+        <v>0</v>
+      </c>
+      <c r="C25" s="75">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="75">
+        <v>0</v>
+      </c>
+      <c r="F25" s="75">
+        <v>1E-3</v>
+      </c>
+      <c r="G25" s="75">
+        <v>1</v>
+      </c>
+      <c r="H25" s="76">
+        <v>1E-8</v>
+      </c>
+      <c r="I25" s="75">
+        <v>0</v>
+      </c>
+      <c r="J25" s="75"/>
+      <c r="K25" s="77" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="75"/>
+      <c r="B26" s="75">
+        <v>1</v>
+      </c>
+      <c r="C26" s="75">
+        <v>0.1</v>
+      </c>
+      <c r="D26" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="75">
+        <v>0</v>
+      </c>
+      <c r="F26" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="G26" s="75">
+        <v>1</v>
+      </c>
+      <c r="H26" s="76">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="I26" s="75">
+        <v>0</v>
+      </c>
+      <c r="J26" s="75"/>
+      <c r="K26" s="77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="75"/>
+      <c r="B27" s="75">
+        <v>3</v>
+      </c>
+      <c r="C27" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="75">
+        <v>0</v>
+      </c>
+      <c r="F27" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="G27" s="75">
+        <v>1</v>
+      </c>
+      <c r="H27" s="76">
+        <v>1E-14</v>
+      </c>
+      <c r="I27" s="75">
+        <v>0</v>
+      </c>
+      <c r="J27" s="75"/>
+      <c r="K27" s="77" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="75"/>
+      <c r="B28" s="75">
+        <v>10</v>
+      </c>
+      <c r="C28" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="D28" s="75">
+        <v>0.97</v>
+      </c>
+      <c r="E28" s="75">
+        <v>0</v>
+      </c>
+      <c r="F28" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="G28" s="75">
+        <v>1</v>
+      </c>
+      <c r="H28" s="76">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I28" s="75">
+        <v>0</v>
+      </c>
+      <c r="J28" s="75"/>
+      <c r="K28" s="77" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="61"/>
+      <c r="B29" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="61"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B33" s="61">
+        <v>12</v>
+      </c>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G34" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H34" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I34" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J34" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K34" s="61"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="75"/>
+      <c r="B35" s="75">
+        <v>0</v>
+      </c>
+      <c r="C35" s="75">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="75">
+        <v>0</v>
+      </c>
+      <c r="F35" s="75">
+        <v>1E-3</v>
+      </c>
+      <c r="G35" s="75">
+        <v>1</v>
+      </c>
+      <c r="H35" s="76">
+        <v>1E-8</v>
+      </c>
+      <c r="I35" s="75">
+        <v>0</v>
+      </c>
+      <c r="J35" s="75"/>
+      <c r="K35" s="77" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="75"/>
+      <c r="B36" s="75">
+        <v>1</v>
+      </c>
+      <c r="C36" s="75">
+        <v>0.1</v>
+      </c>
+      <c r="D36" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="75">
+        <v>0</v>
+      </c>
+      <c r="F36" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="G36" s="75">
+        <v>1</v>
+      </c>
+      <c r="H36" s="76">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="I36" s="75">
+        <v>0</v>
+      </c>
+      <c r="J36" s="75"/>
+      <c r="K36" s="77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="75"/>
+      <c r="B37" s="75">
+        <v>3</v>
+      </c>
+      <c r="C37" s="75">
+        <v>0.6</v>
+      </c>
+      <c r="D37" s="75">
+        <v>0.4</v>
+      </c>
+      <c r="E37" s="75">
+        <v>0</v>
+      </c>
+      <c r="F37" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="G37" s="75">
+        <v>1</v>
+      </c>
+      <c r="H37" s="76">
+        <v>1E-14</v>
+      </c>
+      <c r="I37" s="75">
+        <v>0</v>
+      </c>
+      <c r="J37" s="75"/>
+      <c r="K37" s="77" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="75"/>
+      <c r="B38" s="75">
+        <v>10</v>
+      </c>
+      <c r="C38" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="D38" s="75">
+        <v>0.97</v>
+      </c>
+      <c r="E38" s="75">
+        <v>0</v>
+      </c>
+      <c r="F38" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="G38" s="75">
+        <v>1</v>
+      </c>
+      <c r="H38" s="76">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I38" s="75">
+        <v>0</v>
+      </c>
+      <c r="J38" s="75"/>
+      <c r="K38" s="77" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="61"/>
+      <c r="B39" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="61"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
+      <c r="K42" s="61"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B43" s="61">
+        <v>13</v>
+      </c>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G44" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H44" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I44" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J44" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" s="61"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" s="75"/>
+      <c r="B45" s="75">
+        <v>0</v>
+      </c>
+      <c r="C45" s="75">
+        <v>0.01</v>
+      </c>
+      <c r="D45" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E45" s="75">
+        <v>0</v>
+      </c>
+      <c r="F45" s="75">
+        <v>1E-3</v>
+      </c>
+      <c r="G45" s="75">
+        <v>1</v>
+      </c>
+      <c r="H45" s="76">
+        <v>1E-8</v>
+      </c>
+      <c r="I45" s="75">
+        <v>0</v>
+      </c>
+      <c r="J45" s="75"/>
+      <c r="K45" s="77" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="75"/>
+      <c r="B46" s="75">
+        <v>1</v>
+      </c>
+      <c r="C46" s="75">
+        <v>0.1</v>
+      </c>
+      <c r="D46" s="75">
+        <v>0.5</v>
+      </c>
+      <c r="E46" s="75">
+        <v>0</v>
+      </c>
+      <c r="F46" s="75">
+        <v>0.05</v>
+      </c>
+      <c r="G46" s="75">
+        <v>1</v>
+      </c>
+      <c r="H46" s="76">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="I46" s="75">
+        <v>0</v>
+      </c>
+      <c r="J46" s="75"/>
+      <c r="K46" s="77" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" s="75"/>
+      <c r="B47" s="75">
+        <v>3</v>
+      </c>
+      <c r="C47" s="75">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="75">
+        <v>0.7</v>
+      </c>
+      <c r="E47" s="75">
+        <v>0</v>
+      </c>
+      <c r="F47" s="75">
+        <v>0.15</v>
+      </c>
+      <c r="G47" s="75">
+        <v>1</v>
+      </c>
+      <c r="H47" s="76">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I47" s="75">
+        <v>0</v>
+      </c>
+      <c r="J47" s="75"/>
+      <c r="K47" s="77" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48" s="75"/>
+      <c r="B48" s="75">
+        <v>10</v>
+      </c>
+      <c r="C48" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="D48" s="75">
+        <v>0.97</v>
+      </c>
+      <c r="E48" s="75">
+        <v>0</v>
+      </c>
+      <c r="F48" s="75">
+        <v>0.03</v>
+      </c>
+      <c r="G48" s="75">
+        <v>1</v>
+      </c>
+      <c r="H48" s="76">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I48" s="75">
+        <v>0</v>
+      </c>
+      <c r="J48" s="75"/>
+      <c r="K48" s="77" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="61"/>
+      <c r="B49" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="61"/>
+      <c r="D49" s="61"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+    </row>
+    <row r="54" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A54" s="63" t="s">
+        <v>477</v>
+      </c>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B56" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="61"/>
+      <c r="D56" s="61"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="61"/>
+      <c r="I56" s="61"/>
+      <c r="J56" s="61"/>
+      <c r="K56" s="61"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B57" s="61">
+        <v>21</v>
+      </c>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="61"/>
+      <c r="I57" s="61"/>
+      <c r="J57" s="61"/>
+      <c r="K57" s="61"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="61"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="61"/>
+      <c r="K58" s="61"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G59" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H59" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I59" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J59" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K59" s="61"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60" s="64"/>
+      <c r="B60" s="64">
+        <v>0</v>
+      </c>
+      <c r="C60" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="D60" s="64">
+        <v>0.3</v>
+      </c>
+      <c r="E60" s="64">
+        <v>0</v>
+      </c>
+      <c r="F60" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="G60" s="64">
+        <v>1</v>
+      </c>
+      <c r="H60" s="65">
+        <v>1E-14</v>
+      </c>
+      <c r="I60" s="64">
+        <v>0</v>
+      </c>
+      <c r="J60" s="64"/>
+      <c r="K60" s="66" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61" s="64"/>
+      <c r="B61" s="64">
+        <v>0.05</v>
+      </c>
+      <c r="C61" s="64">
+        <v>0.3</v>
+      </c>
+      <c r="D61" s="64">
+        <v>0.65</v>
+      </c>
+      <c r="E61" s="64">
+        <v>0</v>
+      </c>
+      <c r="F61" s="64">
+        <v>0.2</v>
+      </c>
+      <c r="G61" s="64">
+        <v>2</v>
+      </c>
+      <c r="H61" s="65">
+        <v>1E-14</v>
+      </c>
+      <c r="I61" s="64">
+        <v>0</v>
+      </c>
+      <c r="J61" s="64"/>
+      <c r="K61" s="66" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62" s="64"/>
+      <c r="B62" s="64">
+        <v>3</v>
+      </c>
+      <c r="C62" s="64">
+        <v>0.25</v>
+      </c>
+      <c r="D62" s="64">
+        <v>0.65</v>
+      </c>
+      <c r="E62" s="64">
+        <v>0</v>
+      </c>
+      <c r="F62" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="G62" s="64">
+        <v>2</v>
+      </c>
+      <c r="H62" s="65">
+        <v>1E-14</v>
+      </c>
+      <c r="I62" s="64">
+        <v>0</v>
+      </c>
+      <c r="J62" s="64"/>
+      <c r="K62" s="66" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63" s="64"/>
+      <c r="B63" s="64">
+        <v>10</v>
+      </c>
+      <c r="C63" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="D63" s="64">
+        <v>0.95</v>
+      </c>
+      <c r="E63" s="64">
+        <v>0</v>
+      </c>
+      <c r="F63" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="G63" s="64">
+        <v>1</v>
+      </c>
+      <c r="H63" s="65">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I63" s="64">
+        <v>0</v>
+      </c>
+      <c r="J63" s="64"/>
+      <c r="K63" s="66" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64" s="61"/>
+      <c r="B64" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="61"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="61"/>
+      <c r="E65" s="61"/>
+      <c r="F65" s="61"/>
+      <c r="G65" s="61"/>
+      <c r="H65" s="61"/>
+      <c r="I65" s="61"/>
+      <c r="J65" s="61"/>
+      <c r="K65" s="61"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="61"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="61"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="61"/>
+      <c r="G66" s="61"/>
+      <c r="H66" s="61"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="61"/>
+      <c r="K66" s="61"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="61"/>
+      <c r="F67" s="61"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="61"/>
+      <c r="I67" s="61"/>
+      <c r="J67" s="61"/>
+      <c r="K67" s="61"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B68" s="61">
+        <v>22</v>
+      </c>
+      <c r="C68" s="61"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="61"/>
+      <c r="F68" s="61"/>
+      <c r="G68" s="61"/>
+      <c r="H68" s="61"/>
+      <c r="I68" s="61"/>
+      <c r="J68" s="61"/>
+      <c r="K68" s="61"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="61"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="61"/>
+      <c r="F69" s="61"/>
+      <c r="G69" s="61"/>
+      <c r="H69" s="61"/>
+      <c r="I69" s="61"/>
+      <c r="J69" s="61"/>
+      <c r="K69" s="61"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C70" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F70" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G70" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H70" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I70" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J70" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="61"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="64"/>
+      <c r="B71" s="64">
+        <v>0</v>
+      </c>
+      <c r="C71" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="D71" s="64">
+        <v>0.65</v>
+      </c>
+      <c r="E71" s="64">
+        <v>0</v>
+      </c>
+      <c r="F71" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="G71" s="64">
+        <v>1</v>
+      </c>
+      <c r="H71" s="65">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I71" s="64">
+        <v>0</v>
+      </c>
+      <c r="J71" s="64"/>
+      <c r="K71" s="66" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="64"/>
+      <c r="B72" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="C72" s="64">
+        <v>0.4</v>
+      </c>
+      <c r="D72" s="64">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E72" s="64">
+        <v>0</v>
+      </c>
+      <c r="F72" s="64">
+        <v>0.11</v>
+      </c>
+      <c r="G72" s="64">
+        <v>2</v>
+      </c>
+      <c r="H72" s="65">
+        <v>1E-13</v>
+      </c>
+      <c r="I72" s="64">
+        <v>0</v>
+      </c>
+      <c r="J72" s="64"/>
+      <c r="K72" s="66" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="64"/>
+      <c r="B73" s="64">
+        <v>3</v>
+      </c>
+      <c r="C73" s="64">
+        <v>0.2</v>
+      </c>
+      <c r="D73" s="64">
+        <v>0.7</v>
+      </c>
+      <c r="E73" s="64">
+        <v>0</v>
+      </c>
+      <c r="F73" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="G73" s="64">
+        <v>2</v>
+      </c>
+      <c r="H73" s="65">
+        <v>1E-13</v>
+      </c>
+      <c r="I73" s="64">
+        <v>0</v>
+      </c>
+      <c r="J73" s="64"/>
+      <c r="K73" s="66" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="64"/>
+      <c r="B74" s="64">
+        <v>10</v>
+      </c>
+      <c r="C74" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="D74" s="64">
+        <v>0.97</v>
+      </c>
+      <c r="E74" s="64">
+        <v>0</v>
+      </c>
+      <c r="F74" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="G74" s="64">
+        <v>1</v>
+      </c>
+      <c r="H74" s="65">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I74" s="64">
+        <v>0</v>
+      </c>
+      <c r="J74" s="64"/>
+      <c r="K74" s="66" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="61"/>
+      <c r="B75" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="61"/>
+      <c r="F75" s="61"/>
+      <c r="G75" s="61"/>
+      <c r="H75" s="61"/>
+      <c r="I75" s="61"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="61"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" s="61"/>
+      <c r="C76" s="61"/>
+      <c r="D76" s="61"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
+      <c r="G76" s="61"/>
+      <c r="H76" s="61"/>
+      <c r="I76" s="61"/>
+      <c r="J76" s="61"/>
+      <c r="K76" s="61"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="61"/>
+      <c r="B77" s="61"/>
+      <c r="C77" s="61"/>
+      <c r="D77" s="61"/>
+      <c r="E77" s="61"/>
+      <c r="F77" s="61"/>
+      <c r="G77" s="61"/>
+      <c r="H77" s="61"/>
+      <c r="I77" s="61"/>
+      <c r="J77" s="61"/>
+      <c r="K77" s="61"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="61"/>
+      <c r="D78" s="61"/>
+      <c r="E78" s="61"/>
+      <c r="F78" s="61"/>
+      <c r="G78" s="61"/>
+      <c r="H78" s="61"/>
+      <c r="I78" s="61"/>
+      <c r="J78" s="61"/>
+      <c r="K78" s="61"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B79" s="61">
+        <v>23</v>
+      </c>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="61"/>
+      <c r="H79" s="61"/>
+      <c r="I79" s="61"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="61"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61"/>
+      <c r="J80" s="61"/>
+      <c r="K80" s="61"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A81" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B81" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F81" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G81" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H81" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I81" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J81" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K81" s="61"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82" s="64"/>
+      <c r="B82" s="64">
+        <v>0</v>
+      </c>
+      <c r="C82" s="64">
+        <v>0.05</v>
+      </c>
+      <c r="D82" s="64">
+        <v>0.7</v>
+      </c>
+      <c r="E82" s="64">
+        <v>0</v>
+      </c>
+      <c r="F82" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="G82" s="64">
+        <v>1</v>
+      </c>
+      <c r="H82" s="65">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I82" s="64">
+        <v>0</v>
+      </c>
+      <c r="J82" s="64"/>
+      <c r="K82" s="66" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" s="64"/>
+      <c r="B83" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="C83" s="64">
+        <v>0.1</v>
+      </c>
+      <c r="D83" s="64">
+        <v>0.75</v>
+      </c>
+      <c r="E83" s="64">
+        <v>0</v>
+      </c>
+      <c r="F83" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="G83" s="64">
+        <v>2</v>
+      </c>
+      <c r="H83" s="65">
+        <v>1E-13</v>
+      </c>
+      <c r="I83" s="64">
+        <v>0</v>
+      </c>
+      <c r="J83" s="64"/>
+      <c r="K83" s="66" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84" s="64"/>
+      <c r="B84" s="64">
+        <v>3</v>
+      </c>
+      <c r="C84" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="D84" s="64">
+        <v>0.75</v>
+      </c>
+      <c r="E84" s="64">
+        <v>0</v>
+      </c>
+      <c r="F84" s="64">
+        <v>0.15</v>
+      </c>
+      <c r="G84" s="64">
+        <v>2</v>
+      </c>
+      <c r="H84" s="65">
+        <v>1E-14</v>
+      </c>
+      <c r="I84" s="64">
+        <v>0</v>
+      </c>
+      <c r="J84" s="64"/>
+      <c r="K84" s="66" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85" s="64"/>
+      <c r="B85" s="64">
+        <v>10</v>
+      </c>
+      <c r="C85" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="D85" s="64">
+        <v>0.97</v>
+      </c>
+      <c r="E85" s="64">
+        <v>0</v>
+      </c>
+      <c r="F85" s="64">
+        <v>0.03</v>
+      </c>
+      <c r="G85" s="64">
+        <v>1</v>
+      </c>
+      <c r="H85" s="65">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I85" s="64">
+        <v>0</v>
+      </c>
+      <c r="J85" s="64"/>
+      <c r="K85" s="66" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86" s="61"/>
+      <c r="B86" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" s="61"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
+      <c r="F86" s="61"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="61"/>
+      <c r="I86" s="61"/>
+      <c r="J86" s="61"/>
+      <c r="K86" s="61"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" s="61"/>
+      <c r="C87" s="61"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
+      <c r="F87" s="61"/>
+      <c r="G87" s="61"/>
+      <c r="H87" s="61"/>
+      <c r="I87" s="61"/>
+      <c r="J87" s="61"/>
+      <c r="K87" s="61"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88" s="61"/>
+      <c r="B88" s="61"/>
+      <c r="C88" s="61"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="61"/>
+      <c r="G88" s="61"/>
+      <c r="H88" s="61"/>
+      <c r="I88" s="61"/>
+      <c r="J88" s="61"/>
+      <c r="K88" s="61"/>
+    </row>
+    <row r="90" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A90" s="72" t="s">
+        <v>492</v>
+      </c>
+      <c r="B90" s="72"/>
+      <c r="C90" s="72"/>
+      <c r="D90" s="72"/>
+      <c r="E90" s="72"/>
+      <c r="F90" s="72"/>
+      <c r="G90" s="72"/>
+      <c r="H90" s="72"/>
+      <c r="I90" s="72"/>
+      <c r="J90" s="72"/>
+      <c r="K90" s="72"/>
+    </row>
+    <row r="91" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A91" s="68"/>
+      <c r="B91" s="68"/>
+      <c r="C91" s="68"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="68"/>
+      <c r="G91" s="68"/>
+      <c r="H91" s="68"/>
+      <c r="I91" s="68"/>
+      <c r="J91" s="68"/>
+      <c r="K91" s="68"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="61"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="61"/>
+      <c r="F92" s="61"/>
+      <c r="G92" s="61"/>
+      <c r="H92" s="61"/>
+      <c r="I92" s="61"/>
+      <c r="J92" s="61"/>
+      <c r="K92" s="61"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B93" s="61">
+        <v>24</v>
+      </c>
+      <c r="C93" s="61"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="61"/>
+      <c r="H93" s="61"/>
+      <c r="I93" s="61"/>
+      <c r="J93" s="61"/>
+      <c r="K93" s="61"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="61"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
+      <c r="K94" s="61"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C95" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D95" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E95" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F95" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G95" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H95" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I95" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J95" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K95" s="61"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="81"/>
+      <c r="B96" s="81">
+        <v>0</v>
+      </c>
+      <c r="C96" s="81">
+        <v>0.3</v>
+      </c>
+      <c r="D96" s="81">
+        <v>0.7</v>
+      </c>
+      <c r="E96" s="81">
+        <v>0</v>
+      </c>
+      <c r="F96" s="81">
+        <v>0.25</v>
+      </c>
+      <c r="G96" s="81">
+        <v>2</v>
+      </c>
+      <c r="H96" s="82">
+        <v>1E-14</v>
+      </c>
+      <c r="I96" s="81">
+        <v>0</v>
+      </c>
+      <c r="J96" s="81"/>
+      <c r="K96" s="83" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="81"/>
+      <c r="B97" s="81">
+        <v>1</v>
+      </c>
+      <c r="C97" s="81">
+        <v>0.25</v>
+      </c>
+      <c r="D97" s="81">
+        <v>0.7</v>
+      </c>
+      <c r="E97" s="81">
+        <v>0</v>
+      </c>
+      <c r="F97" s="81">
+        <v>0.2</v>
+      </c>
+      <c r="G97" s="81">
+        <v>2</v>
+      </c>
+      <c r="H97" s="82">
+        <v>1E-13</v>
+      </c>
+      <c r="I97" s="81">
+        <v>0</v>
+      </c>
+      <c r="J97" s="81"/>
+      <c r="K97" s="83" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="81"/>
+      <c r="B98" s="81">
+        <v>5</v>
+      </c>
+      <c r="C98" s="81">
+        <v>0.25</v>
+      </c>
+      <c r="D98" s="81">
+        <v>0.7</v>
+      </c>
+      <c r="E98" s="81">
+        <v>0</v>
+      </c>
+      <c r="F98" s="81">
+        <v>0.1</v>
+      </c>
+      <c r="G98" s="81">
+        <v>2</v>
+      </c>
+      <c r="H98" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I98" s="81"/>
+      <c r="J98" s="81"/>
+      <c r="K98" s="83" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99" s="81"/>
+      <c r="B99" s="81">
+        <v>10</v>
+      </c>
+      <c r="C99" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="D99" s="81">
+        <v>0.97</v>
+      </c>
+      <c r="E99" s="81">
+        <v>0</v>
+      </c>
+      <c r="F99" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="G99" s="81">
+        <v>1</v>
+      </c>
+      <c r="H99" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I99" s="81">
+        <v>0</v>
+      </c>
+      <c r="J99" s="81"/>
+      <c r="K99" s="83" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="61"/>
+      <c r="B100" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100" s="61"/>
+      <c r="D100" s="61"/>
+      <c r="E100" s="61"/>
+      <c r="F100" s="61"/>
+      <c r="G100" s="61"/>
+      <c r="H100" s="61"/>
+      <c r="I100" s="61"/>
+      <c r="J100" s="61"/>
+      <c r="K100" s="61"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="61"/>
+      <c r="C101" s="61"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="61"/>
+      <c r="F101" s="61"/>
+      <c r="G101" s="61"/>
+      <c r="H101" s="61"/>
+      <c r="I101" s="61"/>
+      <c r="J101" s="61"/>
+      <c r="K101" s="61"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="61"/>
+      <c r="B102" s="61"/>
+      <c r="C102" s="61"/>
+      <c r="D102" s="61"/>
+      <c r="E102" s="61"/>
+      <c r="F102" s="61"/>
+      <c r="G102" s="61"/>
+      <c r="H102" s="61"/>
+      <c r="I102" s="61"/>
+      <c r="J102" s="61"/>
+      <c r="K102" s="61"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B103" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" s="61"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="61"/>
+      <c r="F103" s="61"/>
+      <c r="G103" s="61"/>
+      <c r="H103" s="61"/>
+      <c r="I103" s="61"/>
+      <c r="J103" s="61"/>
+      <c r="K103" s="61"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B104" s="61">
+        <v>25</v>
+      </c>
+      <c r="C104" s="61"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="61"/>
+      <c r="G104" s="61"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="61"/>
+      <c r="J104" s="61"/>
+      <c r="K104" s="61"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B105" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D105" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E105" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F105" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G105" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H105" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I105" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J105" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K105" s="61"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="81"/>
+      <c r="B106" s="81">
+        <v>0</v>
+      </c>
+      <c r="C106" s="81">
+        <v>0.3</v>
+      </c>
+      <c r="D106" s="81">
+        <v>0.7</v>
+      </c>
+      <c r="E106" s="81">
+        <v>0</v>
+      </c>
+      <c r="F106" s="81">
+        <v>0.25</v>
+      </c>
+      <c r="G106" s="81">
+        <v>2</v>
+      </c>
+      <c r="H106" s="82">
+        <v>1E-14</v>
+      </c>
+      <c r="I106" s="81">
+        <v>0</v>
+      </c>
+      <c r="J106" s="81"/>
+      <c r="K106" s="83" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107" s="81"/>
+      <c r="B107" s="81">
+        <v>0.3</v>
+      </c>
+      <c r="C107" s="81">
+        <v>0.2</v>
+      </c>
+      <c r="D107" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="E107" s="81">
+        <v>0</v>
+      </c>
+      <c r="F107" s="81">
+        <v>0.2</v>
+      </c>
+      <c r="G107" s="81">
+        <v>2</v>
+      </c>
+      <c r="H107" s="82">
+        <v>1E-13</v>
+      </c>
+      <c r="I107" s="81">
+        <v>0</v>
+      </c>
+      <c r="J107" s="81"/>
+      <c r="K107" s="83" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A108" s="81"/>
+      <c r="B108" s="81">
+        <v>2</v>
+      </c>
+      <c r="C108" s="81">
+        <v>0.1</v>
+      </c>
+      <c r="D108" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E108" s="81">
+        <v>0</v>
+      </c>
+      <c r="F108" s="81">
+        <v>0.1</v>
+      </c>
+      <c r="G108" s="81">
+        <v>2</v>
+      </c>
+      <c r="H108" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I108" s="81">
+        <v>0</v>
+      </c>
+      <c r="J108" s="81"/>
+      <c r="K108" s="83"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A109" s="81"/>
+      <c r="B109" s="81">
+        <v>10</v>
+      </c>
+      <c r="C109" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="D109" s="81">
+        <v>0.97</v>
+      </c>
+      <c r="E109" s="81">
+        <v>0</v>
+      </c>
+      <c r="F109" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="G109" s="81">
+        <v>1</v>
+      </c>
+      <c r="H109" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I109" s="81">
+        <v>0</v>
+      </c>
+      <c r="J109" s="81"/>
+      <c r="K109" s="83"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A110" s="61"/>
+      <c r="B110" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="61"/>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
+      <c r="F110" s="61"/>
+      <c r="G110" s="61"/>
+      <c r="H110" s="61"/>
+      <c r="I110" s="61"/>
+      <c r="J110" s="61"/>
+      <c r="K110" s="61"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A111" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="61"/>
+      <c r="C111" s="61"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="61"/>
+      <c r="F111" s="61"/>
+      <c r="G111" s="61"/>
+      <c r="H111" s="61"/>
+      <c r="I111" s="61"/>
+      <c r="J111" s="61"/>
+      <c r="K111" s="61"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="61"/>
+      <c r="B112" s="61"/>
+      <c r="C112" s="61"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="61"/>
+      <c r="F112" s="61"/>
+      <c r="G112" s="61"/>
+      <c r="H112" s="61"/>
+      <c r="I112" s="61"/>
+      <c r="J112" s="61"/>
+      <c r="K112" s="61"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A113" s="61"/>
+      <c r="B113" s="61"/>
+      <c r="C113" s="61"/>
+      <c r="D113" s="61"/>
+      <c r="E113" s="61"/>
+      <c r="F113" s="61"/>
+      <c r="G113" s="61"/>
+      <c r="H113" s="61"/>
+      <c r="I113" s="61"/>
+      <c r="J113" s="61"/>
+      <c r="K113" s="61"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="61"/>
+      <c r="D114" s="61"/>
+      <c r="E114" s="61"/>
+      <c r="F114" s="61"/>
+      <c r="G114" s="61"/>
+      <c r="H114" s="61"/>
+      <c r="I114" s="61"/>
+      <c r="J114" s="61"/>
+      <c r="K114" s="61"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A115" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B115" s="61">
+        <v>26</v>
+      </c>
+      <c r="C115" s="61"/>
+      <c r="D115" s="61"/>
+      <c r="E115" s="61"/>
+      <c r="F115" s="61"/>
+      <c r="G115" s="61"/>
+      <c r="H115" s="61"/>
+      <c r="I115" s="61"/>
+      <c r="J115" s="61"/>
+      <c r="K115" s="61"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A116" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B116" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D116" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E116" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F116" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G116" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H116" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I116" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J116" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K116" s="61"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="81"/>
+      <c r="B117" s="81">
+        <v>0</v>
+      </c>
+      <c r="C117" s="81">
+        <v>0.2</v>
+      </c>
+      <c r="D117" s="81">
+        <v>0.75</v>
+      </c>
+      <c r="E117" s="81">
+        <v>0</v>
+      </c>
+      <c r="F117" s="81">
+        <v>0.2</v>
+      </c>
+      <c r="G117" s="81">
+        <v>2</v>
+      </c>
+      <c r="H117" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I117" s="81">
+        <v>0</v>
+      </c>
+      <c r="J117" s="81"/>
+      <c r="K117" s="83" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="81"/>
+      <c r="B118" s="81">
+        <v>3</v>
+      </c>
+      <c r="C118" s="81">
+        <v>0.1</v>
+      </c>
+      <c r="D118" s="81">
+        <v>0.85</v>
+      </c>
+      <c r="E118" s="81">
+        <v>0</v>
+      </c>
+      <c r="F118" s="81">
+        <v>0.15</v>
+      </c>
+      <c r="G118" s="81">
+        <v>2</v>
+      </c>
+      <c r="H118" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I118" s="81">
+        <v>0</v>
+      </c>
+      <c r="J118" s="81"/>
+      <c r="K118" s="83"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="81"/>
+      <c r="B119" s="81">
+        <v>10</v>
+      </c>
+      <c r="C119" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="D119" s="81">
+        <v>0.97</v>
+      </c>
+      <c r="E119" s="81">
+        <v>0</v>
+      </c>
+      <c r="F119" s="81">
+        <v>0.03</v>
+      </c>
+      <c r="G119" s="81">
+        <v>1</v>
+      </c>
+      <c r="H119" s="82">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I119" s="81">
+        <v>0</v>
+      </c>
+      <c r="J119" s="81"/>
+      <c r="K119" s="83"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A120" s="61"/>
+      <c r="B120" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C120" s="61"/>
+      <c r="D120" s="61"/>
+      <c r="E120" s="61"/>
+      <c r="F120" s="61"/>
+      <c r="G120" s="61"/>
+      <c r="H120" s="61"/>
+      <c r="I120" s="61"/>
+      <c r="J120" s="61"/>
+      <c r="K120" s="61"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A121" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" s="61"/>
+      <c r="C121" s="61"/>
+      <c r="D121" s="61"/>
+      <c r="E121" s="61"/>
+      <c r="F121" s="61"/>
+      <c r="G121" s="61"/>
+      <c r="H121" s="61"/>
+      <c r="I121" s="61"/>
+      <c r="J121" s="61"/>
+      <c r="K121" s="61"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A122" s="61"/>
+      <c r="B122" s="61"/>
+      <c r="C122" s="61"/>
+      <c r="D122" s="61"/>
+      <c r="E122" s="61"/>
+      <c r="F122" s="61"/>
+      <c r="G122" s="61"/>
+      <c r="H122" s="61"/>
+      <c r="I122" s="61"/>
+      <c r="J122" s="61"/>
+      <c r="K122" s="61"/>
+    </row>
+    <row r="124" spans="1:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="A124" s="60" t="s">
+        <v>462</v>
+      </c>
+      <c r="B124" s="60"/>
+      <c r="C124" s="60"/>
+      <c r="D124" s="60"/>
+      <c r="E124" s="60"/>
+      <c r="F124" s="60"/>
+      <c r="G124" s="60"/>
+      <c r="H124" s="60"/>
+      <c r="I124" s="60"/>
+      <c r="J124" s="60"/>
+      <c r="K124" s="60"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A126" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="61"/>
+      <c r="D126" s="61"/>
+      <c r="E126" s="61"/>
+      <c r="F126" s="61"/>
+      <c r="G126" s="61"/>
+      <c r="H126" s="61"/>
+      <c r="I126" s="61"/>
+      <c r="J126" s="61"/>
+      <c r="K126" s="61"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A127" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B127" s="61">
+        <v>31</v>
+      </c>
+      <c r="C127" s="61"/>
+      <c r="D127" s="61"/>
+      <c r="E127" s="61"/>
+      <c r="F127" s="61"/>
+      <c r="G127" s="61"/>
+      <c r="H127" s="61"/>
+      <c r="I127" s="61"/>
+      <c r="J127" s="61"/>
+      <c r="K127" s="61"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A128" s="61"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="61"/>
+      <c r="D128" s="61"/>
+      <c r="E128" s="61"/>
+      <c r="F128" s="61"/>
+      <c r="G128" s="61"/>
+      <c r="H128" s="61"/>
+      <c r="I128" s="61"/>
+      <c r="J128" s="61"/>
+      <c r="K128" s="61"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B129" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C129" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D129" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E129" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F129" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G129" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H129" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I129" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J129" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K129" s="61"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A130" s="78"/>
+      <c r="B130" s="78">
+        <v>0</v>
+      </c>
+      <c r="C130" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="D130" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="E130" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="F130" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="G130" s="78">
+        <v>1</v>
+      </c>
+      <c r="H130" s="79">
+        <v>1E-14</v>
+      </c>
+      <c r="I130" s="78">
+        <v>0</v>
+      </c>
+      <c r="J130" s="78"/>
+      <c r="K130" s="80" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A131" s="78"/>
+      <c r="B131" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="C131" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="D131" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="E131" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="F131" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G131" s="78">
+        <v>2</v>
+      </c>
+      <c r="H131" s="79">
+        <v>1E-14</v>
+      </c>
+      <c r="I131" s="78">
+        <v>0</v>
+      </c>
+      <c r="J131" s="78"/>
+      <c r="K131" s="80" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="78"/>
+      <c r="B132" s="78">
+        <v>1</v>
+      </c>
+      <c r="C132" s="78">
+        <v>0.25</v>
+      </c>
+      <c r="D132" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="E132" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="F132" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G132" s="78">
+        <v>2</v>
+      </c>
+      <c r="H132" s="79">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I132" s="78">
+        <v>0</v>
+      </c>
+      <c r="J132" s="78"/>
+      <c r="K132" s="80" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="78"/>
+      <c r="B133" s="78">
+        <v>10</v>
+      </c>
+      <c r="C133" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="D133" s="78">
+        <v>0.97</v>
+      </c>
+      <c r="E133" s="78">
+        <v>0</v>
+      </c>
+      <c r="F133" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="G133" s="78">
+        <v>1</v>
+      </c>
+      <c r="H133" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I133" s="78">
+        <v>0</v>
+      </c>
+      <c r="J133" s="78"/>
+      <c r="K133" s="80" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A134" s="61"/>
+      <c r="B134" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C134" s="61"/>
+      <c r="D134" s="61"/>
+      <c r="E134" s="61"/>
+      <c r="F134" s="61"/>
+      <c r="G134" s="61"/>
+      <c r="H134" s="61"/>
+      <c r="I134" s="61"/>
+      <c r="J134" s="61"/>
+      <c r="K134" s="61"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A135" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="61"/>
+      <c r="C135" s="61"/>
+      <c r="D135" s="61"/>
+      <c r="E135" s="61"/>
+      <c r="F135" s="61"/>
+      <c r="G135" s="61"/>
+      <c r="H135" s="61"/>
+      <c r="I135" s="61"/>
+      <c r="J135" s="61"/>
+      <c r="K135" s="61"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A136" s="61"/>
+      <c r="B136" s="61"/>
+      <c r="C136" s="61"/>
+      <c r="D136" s="61"/>
+      <c r="E136" s="61"/>
+      <c r="F136" s="61"/>
+      <c r="G136" s="61"/>
+      <c r="H136" s="61"/>
+      <c r="I136" s="61"/>
+      <c r="J136" s="61"/>
+      <c r="K136" s="61"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A137" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B137" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="61"/>
+      <c r="D137" s="61"/>
+      <c r="E137" s="61"/>
+      <c r="F137" s="61"/>
+      <c r="G137" s="61"/>
+      <c r="H137" s="61"/>
+      <c r="I137" s="61"/>
+      <c r="J137" s="61"/>
+      <c r="K137" s="61"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B138" s="61">
+        <v>32</v>
+      </c>
+      <c r="C138" s="61"/>
+      <c r="D138" s="61"/>
+      <c r="E138" s="61"/>
+      <c r="F138" s="61"/>
+      <c r="G138" s="61"/>
+      <c r="H138" s="61"/>
+      <c r="I138" s="61"/>
+      <c r="J138" s="61"/>
+      <c r="K138" s="61"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B139" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C139" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D139" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E139" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F139" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G139" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H139" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I139" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J139" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K139" s="61"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" s="78"/>
+      <c r="B140" s="78">
+        <v>0</v>
+      </c>
+      <c r="C140" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="D140" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="E140" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="F140" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G140" s="78">
+        <v>1</v>
+      </c>
+      <c r="H140" s="79">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I140" s="78">
+        <v>0</v>
+      </c>
+      <c r="J140" s="78"/>
+      <c r="K140" s="80" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" s="78"/>
+      <c r="B141" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="C141" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="D141" s="78">
+        <v>0.4</v>
+      </c>
+      <c r="E141" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="F141" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="G141" s="78">
+        <v>2</v>
+      </c>
+      <c r="H141" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I141" s="78">
+        <v>0</v>
+      </c>
+      <c r="J141" s="78"/>
+      <c r="K141" s="80" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" s="78"/>
+      <c r="B142" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="C142" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="D142" s="78">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E142" s="78">
+        <v>0</v>
+      </c>
+      <c r="F142" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="G142" s="78">
+        <v>2</v>
+      </c>
+      <c r="H142" s="79">
+        <v>1E-13</v>
+      </c>
+      <c r="I142" s="78">
+        <v>0</v>
+      </c>
+      <c r="J142" s="78"/>
+      <c r="K142" s="80" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" s="78"/>
+      <c r="B143" s="78">
+        <v>1</v>
+      </c>
+      <c r="C143" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="D143" s="78">
+        <v>0.75</v>
+      </c>
+      <c r="E143" s="78">
+        <v>0</v>
+      </c>
+      <c r="F143" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G143" s="78">
+        <v>2</v>
+      </c>
+      <c r="H143" s="79">
+        <v>1E-13</v>
+      </c>
+      <c r="I143" s="78">
+        <v>0</v>
+      </c>
+      <c r="J143" s="78"/>
+      <c r="K143" s="80" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" s="78"/>
+      <c r="B144" s="78">
+        <v>10</v>
+      </c>
+      <c r="C144" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="D144" s="78">
+        <v>0.97</v>
+      </c>
+      <c r="E144" s="78">
+        <v>0</v>
+      </c>
+      <c r="F144" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="G144" s="78">
+        <v>1</v>
+      </c>
+      <c r="H144" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I144" s="78">
+        <v>0</v>
+      </c>
+      <c r="J144" s="78"/>
+      <c r="K144" s="80" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" s="61"/>
+      <c r="B145" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C145" s="61"/>
+      <c r="D145" s="61"/>
+      <c r="E145" s="61"/>
+      <c r="F145" s="61"/>
+      <c r="G145" s="61"/>
+      <c r="H145" s="61"/>
+      <c r="I145" s="61"/>
+      <c r="J145" s="61"/>
+      <c r="K145" s="61"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" s="61"/>
+      <c r="C146" s="61"/>
+      <c r="D146" s="61"/>
+      <c r="E146" s="61"/>
+      <c r="F146" s="61"/>
+      <c r="G146" s="61"/>
+      <c r="H146" s="61"/>
+      <c r="I146" s="61"/>
+      <c r="J146" s="61"/>
+      <c r="K146" s="61"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" s="61"/>
+      <c r="B147" s="61"/>
+      <c r="C147" s="61"/>
+      <c r="D147" s="61"/>
+      <c r="E147" s="61"/>
+      <c r="F147" s="61"/>
+      <c r="G147" s="61"/>
+      <c r="H147" s="61"/>
+      <c r="I147" s="61"/>
+      <c r="J147" s="61"/>
+      <c r="K147" s="61"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" s="61"/>
+      <c r="B148" s="61"/>
+      <c r="C148" s="61"/>
+      <c r="D148" s="61"/>
+      <c r="E148" s="61"/>
+      <c r="F148" s="61"/>
+      <c r="G148" s="61"/>
+      <c r="H148" s="61"/>
+      <c r="I148" s="61"/>
+      <c r="J148" s="61"/>
+      <c r="K148" s="61"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B149" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149" s="61"/>
+      <c r="D149" s="61"/>
+      <c r="E149" s="61"/>
+      <c r="F149" s="61"/>
+      <c r="G149" s="61"/>
+      <c r="H149" s="61"/>
+      <c r="I149" s="61"/>
+      <c r="J149" s="61"/>
+      <c r="K149" s="61"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A150" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B150" s="61">
+        <v>33</v>
+      </c>
+      <c r="C150" s="61"/>
+      <c r="D150" s="61"/>
+      <c r="E150" s="61"/>
+      <c r="F150" s="61"/>
+      <c r="G150" s="61"/>
+      <c r="H150" s="61"/>
+      <c r="I150" s="61"/>
+      <c r="J150" s="61"/>
+      <c r="K150" s="61"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A151" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B151" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C151" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D151" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E151" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F151" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G151" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H151" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I151" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J151" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K151" s="61"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A152" s="78"/>
+      <c r="B152" s="78">
+        <v>0</v>
+      </c>
+      <c r="C152" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="D152" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="E152" s="78">
+        <v>0.5</v>
+      </c>
+      <c r="F152" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G152" s="78">
+        <v>1</v>
+      </c>
+      <c r="H152" s="79">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I152" s="78">
+        <v>0</v>
+      </c>
+      <c r="J152" s="78"/>
+      <c r="K152" s="80" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A153" s="78"/>
+      <c r="B153" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="C153" s="78">
+        <v>0.3</v>
+      </c>
+      <c r="D153" s="78">
+        <v>0.5</v>
+      </c>
+      <c r="E153" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="F153" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="G153" s="78">
+        <v>2</v>
+      </c>
+      <c r="H153" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I153" s="78">
+        <v>0</v>
+      </c>
+      <c r="J153" s="78"/>
+      <c r="K153" s="80" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A154" s="78"/>
+      <c r="B154" s="78">
+        <v>3</v>
+      </c>
+      <c r="C154" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="D154" s="78">
+        <v>0.75</v>
+      </c>
+      <c r="E154" s="78">
+        <v>0</v>
+      </c>
+      <c r="F154" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="G154" s="78">
+        <v>2</v>
+      </c>
+      <c r="H154" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I154" s="78">
+        <v>0</v>
+      </c>
+      <c r="J154" s="78"/>
+      <c r="K154" s="80" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A155" s="78"/>
+      <c r="B155" s="78">
+        <v>10</v>
+      </c>
+      <c r="C155" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="D155" s="78">
+        <v>0.97</v>
+      </c>
+      <c r="E155" s="78">
+        <v>0</v>
+      </c>
+      <c r="F155" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="G155" s="78">
+        <v>1</v>
+      </c>
+      <c r="H155" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I155" s="78">
+        <v>0</v>
+      </c>
+      <c r="J155" s="78"/>
+      <c r="K155" s="80" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A156" s="61"/>
+      <c r="B156" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C156" s="61"/>
+      <c r="D156" s="61"/>
+      <c r="E156" s="61"/>
+      <c r="F156" s="61"/>
+      <c r="G156" s="61"/>
+      <c r="H156" s="61"/>
+      <c r="I156" s="61"/>
+      <c r="J156" s="61"/>
+      <c r="K156" s="61"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A157" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" s="61"/>
+      <c r="C157" s="61"/>
+      <c r="D157" s="61"/>
+      <c r="E157" s="61"/>
+      <c r="F157" s="61"/>
+      <c r="G157" s="61"/>
+      <c r="H157" s="61"/>
+      <c r="I157" s="61"/>
+      <c r="J157" s="61"/>
+      <c r="K157" s="61"/>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A158" s="61"/>
+      <c r="B158" s="61"/>
+      <c r="C158" s="61"/>
+      <c r="D158" s="61"/>
+      <c r="E158" s="61"/>
+      <c r="F158" s="61"/>
+      <c r="G158" s="61"/>
+      <c r="H158" s="61"/>
+      <c r="I158" s="61"/>
+      <c r="J158" s="61"/>
+      <c r="K158" s="61"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A159" s="61"/>
+      <c r="B159" s="61"/>
+      <c r="C159" s="61"/>
+      <c r="D159" s="61"/>
+      <c r="E159" s="61"/>
+      <c r="F159" s="61"/>
+      <c r="G159" s="61"/>
+      <c r="H159" s="61"/>
+      <c r="I159" s="61"/>
+      <c r="J159" s="61"/>
+      <c r="K159" s="61"/>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A160" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B160" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160" s="61"/>
+      <c r="D160" s="61"/>
+      <c r="E160" s="61"/>
+      <c r="F160" s="61"/>
+      <c r="G160" s="61"/>
+      <c r="H160" s="61"/>
+      <c r="I160" s="61"/>
+      <c r="J160" s="61"/>
+      <c r="K160" s="61"/>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A161" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="B161" s="61">
+        <v>34</v>
+      </c>
+      <c r="C161" s="61" t="s">
+        <v>476</v>
+      </c>
+      <c r="D161" s="61"/>
+      <c r="E161" s="61"/>
+      <c r="F161" s="61"/>
+      <c r="G161" s="61"/>
+      <c r="H161" s="61"/>
+      <c r="I161" s="61"/>
+      <c r="J161" s="61"/>
+      <c r="K161" s="61"/>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A162" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B162" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="C162" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="D162" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E162" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F162" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G162" s="62" t="s">
+        <v>244</v>
+      </c>
+      <c r="H162" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="I162" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="J162" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="K162" s="61"/>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A163" s="78"/>
+      <c r="B163" s="78">
+        <v>0</v>
+      </c>
+      <c r="C163" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="D163" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="E163" s="78">
+        <v>0.5</v>
+      </c>
+      <c r="F163" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G163" s="78">
+        <v>1</v>
+      </c>
+      <c r="H163" s="79">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="I163" s="78">
+        <v>0</v>
+      </c>
+      <c r="J163" s="78"/>
+      <c r="K163" s="80" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A164" s="78"/>
+      <c r="B164" s="78">
+        <v>0.05</v>
+      </c>
+      <c r="C164" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="D164" s="78">
+        <v>0.6</v>
+      </c>
+      <c r="E164" s="78">
+        <v>0.2</v>
+      </c>
+      <c r="F164" s="78">
+        <v>0.15</v>
+      </c>
+      <c r="G164" s="78">
+        <v>2</v>
+      </c>
+      <c r="H164" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I164" s="78">
+        <v>0</v>
+      </c>
+      <c r="J164" s="78"/>
+      <c r="K164" s="80" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A165" s="78"/>
+      <c r="B165" s="78">
+        <v>3</v>
+      </c>
+      <c r="C165" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="D165" s="78">
+        <v>0.8</v>
+      </c>
+      <c r="E165" s="78">
+        <v>0</v>
+      </c>
+      <c r="F165" s="78">
+        <v>0.1</v>
+      </c>
+      <c r="G165" s="78">
+        <v>2</v>
+      </c>
+      <c r="H165" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I165" s="78">
+        <v>0</v>
+      </c>
+      <c r="J165" s="78"/>
+      <c r="K165" s="80" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A166" s="78"/>
+      <c r="B166" s="78">
+        <v>10</v>
+      </c>
+      <c r="C166" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="D166" s="78">
+        <v>0.97</v>
+      </c>
+      <c r="E166" s="78">
+        <v>0</v>
+      </c>
+      <c r="F166" s="78">
+        <v>0.03</v>
+      </c>
+      <c r="G166" s="78">
+        <v>1</v>
+      </c>
+      <c r="H166" s="79">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="I166" s="78">
+        <v>0</v>
+      </c>
+      <c r="J166" s="78"/>
+      <c r="K166" s="80" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B167" t="s">
+        <v>26</v>
+      </c>
+      <c r="C167" s="61"/>
+      <c r="D167" s="61"/>
+      <c r="E167" s="61"/>
+      <c r="F167" s="61"/>
+      <c r="G167" s="61"/>
+      <c r="H167" s="61"/>
+      <c r="I167" s="61"/>
+      <c r="J167" s="61"/>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A170" s="61"/>
+      <c r="B170" s="61"/>
+      <c r="C170" s="61"/>
+      <c r="D170" s="61"/>
+      <c r="E170" s="61"/>
+      <c r="F170" s="61"/>
+      <c r="G170" s="61"/>
+      <c r="H170" s="61"/>
+      <c r="I170" s="61"/>
+      <c r="J170" s="61"/>
+      <c r="K170" s="61"/>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A171" s="61"/>
+      <c r="B171" s="61"/>
+      <c r="C171" s="61"/>
+      <c r="D171" s="61"/>
+      <c r="E171" s="61"/>
+      <c r="F171" s="61"/>
+      <c r="G171" s="61"/>
+      <c r="H171" s="61"/>
+      <c r="I171" s="61"/>
+      <c r="J171" s="61"/>
+      <c r="K171" s="61"/>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A172" s="61"/>
+      <c r="B172" s="61"/>
+      <c r="C172" s="61"/>
+      <c r="D172" s="61"/>
+      <c r="E172" s="61"/>
+      <c r="F172" s="61"/>
+      <c r="G172" s="61"/>
+      <c r="H172" s="61"/>
+      <c r="I172" s="61"/>
+      <c r="J172" s="61"/>
+      <c r="K172" s="61"/>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A173" s="61"/>
+      <c r="B173" s="61"/>
+      <c r="C173" s="61"/>
+      <c r="D173" s="61"/>
+      <c r="E173" s="61"/>
+      <c r="F173" s="61"/>
+      <c r="G173" s="61"/>
+      <c r="H173" s="61"/>
+      <c r="I173" s="61"/>
+      <c r="J173" s="61"/>
+      <c r="K173" s="61"/>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A174" s="61"/>
+      <c r="B174" s="61"/>
+      <c r="C174" s="61"/>
+      <c r="D174" s="61"/>
+      <c r="E174" s="61"/>
+      <c r="F174" s="61"/>
+      <c r="G174" s="61"/>
+      <c r="H174" s="61"/>
+      <c r="I174" s="61"/>
+      <c r="J174" s="61"/>
+      <c r="K174" s="61"/>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A175" s="61"/>
+      <c r="B175" s="61"/>
+      <c r="C175" s="61"/>
+      <c r="D175" s="61"/>
+      <c r="E175" s="61"/>
+      <c r="F175" s="61"/>
+      <c r="G175" s="61"/>
+      <c r="H175" s="61"/>
+      <c r="I175" s="61"/>
+      <c r="J175" s="61"/>
+      <c r="K175" s="61"/>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A176" s="61"/>
+      <c r="B176" s="61"/>
+      <c r="C176" s="61"/>
+      <c r="D176" s="61"/>
+      <c r="E176" s="61"/>
+      <c r="F176" s="61"/>
+      <c r="G176" s="61"/>
+      <c r="H176" s="61"/>
+      <c r="I176" s="61"/>
+      <c r="J176" s="61"/>
+      <c r="K176" s="61"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA10F18-5214-574C-919F-C3B3EBAFB4FF}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -8144,7 +12019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F382DC3-FE01-C145-884F-393A662961F2}">
   <dimension ref="A1:AE1003"/>
   <sheetViews>

</xml_diff>